<commit_message>
Added Rotation Methods for Cartesian Coordinates
Added Rotation Methods for Cartesian Coordinates
</commit_message>
<xml_diff>
--- a/docs/Math Tests.xlsx
+++ b/docs/Math Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\personal\MPT.Net\MPT\Math\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FF30F5-1710-4E45-8267-DAEA0A01CA2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F13126A-F0F9-4937-815A-5ED16E28F82A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="824" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="824" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Numbers" sheetId="3" r:id="rId1"/>
@@ -26,22 +26,22 @@
     <sheet name="Vectors" sheetId="10" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="a_2" localSheetId="1">Algebra!$C$349</definedName>
-    <definedName name="a_bar" localSheetId="1">Algebra!$C$256</definedName>
-    <definedName name="A_cap" localSheetId="1">Algebra!$C$260</definedName>
-    <definedName name="b_bar" localSheetId="1">Algebra!$C$257</definedName>
-    <definedName name="B_cap" localSheetId="1">Algebra!$C$261</definedName>
-    <definedName name="c_bar" localSheetId="1">Algebra!$C$258</definedName>
-    <definedName name="d_bar" localSheetId="1">Algebra!$C$259</definedName>
-    <definedName name="F_e22" localSheetId="1">Algebra!$C$342</definedName>
-    <definedName name="F_e33" localSheetId="1">Algebra!$C$343</definedName>
-    <definedName name="F_ez" localSheetId="1">Algebra!$C$344</definedName>
-    <definedName name="Q" localSheetId="1">Algebra!$C$352</definedName>
-    <definedName name="r_o" localSheetId="1">Algebra!$C$104</definedName>
-    <definedName name="t" localSheetId="1">Algebra!$C$263</definedName>
-    <definedName name="theta" localSheetId="1">Algebra!$C$357</definedName>
-    <definedName name="x_o" localSheetId="1">Algebra!$C$97</definedName>
-    <definedName name="y_o" localSheetId="1">Algebra!$C$101</definedName>
+    <definedName name="a_2" localSheetId="1">Algebra!$C$307</definedName>
+    <definedName name="a_bar" localSheetId="1">Algebra!$C$214</definedName>
+    <definedName name="A_cap" localSheetId="1">Algebra!$C$218</definedName>
+    <definedName name="b_bar" localSheetId="1">Algebra!$C$215</definedName>
+    <definedName name="B_cap" localSheetId="1">Algebra!$C$219</definedName>
+    <definedName name="c_bar" localSheetId="1">Algebra!$C$216</definedName>
+    <definedName name="d_bar" localSheetId="1">Algebra!$C$217</definedName>
+    <definedName name="F_e22" localSheetId="1">Algebra!$C$300</definedName>
+    <definedName name="F_e33" localSheetId="1">Algebra!$C$301</definedName>
+    <definedName name="F_ez" localSheetId="1">Algebra!$C$302</definedName>
+    <definedName name="Q" localSheetId="1">Algebra!$C$310</definedName>
+    <definedName name="r_o" localSheetId="1">Algebra!$C$62</definedName>
+    <definedName name="t" localSheetId="1">Algebra!$C$221</definedName>
+    <definedName name="theta" localSheetId="1">Algebra!$C$315</definedName>
+    <definedName name="x_o" localSheetId="1">Algebra!$C$55</definedName>
+    <definedName name="y_o" localSheetId="1">Algebra!$C$59</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="183">
   <si>
     <t>Cube Root</t>
   </si>
@@ -598,28 +598,16 @@
     <t>T</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>aCosRatio</t>
-  </si>
-  <si>
-    <t>pi/2</t>
-  </si>
-  <si>
-    <t>pi/4</t>
-  </si>
-  <si>
-    <t>pi</t>
-  </si>
-  <si>
-    <t>(3/4)pi</t>
+    <t>Rotate</t>
+  </si>
+  <si>
+    <t>RotateAboutPoint</t>
+  </si>
+  <si>
+    <t>Xcenter</t>
+  </si>
+  <si>
+    <t>Ycenter</t>
   </si>
 </sst>
 </file>
@@ -700,7 +688,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -726,60 +714,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -827,18 +767,6 @@
     <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2414,10 +2342,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P66"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3243,404 +3171,6 @@
       <c r="P26" t="str">
         <f>"[TestCase("&amp;ROUND(A26,6)&amp;", "&amp;ROUND(B26,6)&amp;", "&amp;ROUND(C26,6)&amp;", "&amp;ROUND(D26,6)&amp;", "&amp;ROUND(L26,6)&amp;", "&amp;ROUND(M26,6)&amp;", "&amp;ROUND(N26,6)&amp;")]"</f>
         <v>[TestCase(0.636733, -378.604263, 59057.623334, -1627072.644858, 351.26821, 34.90111, 208.435572)]</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="41"/>
-      <c r="B30" s="42" t="s">
-        <v>179</v>
-      </c>
-      <c r="C30" s="42" t="s">
-        <v>180</v>
-      </c>
-      <c r="D30" s="42" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="43"/>
-      <c r="B31" s="44" t="s">
-        <v>182</v>
-      </c>
-      <c r="C31" s="44">
-        <v>-2.3380354754055399</v>
-      </c>
-      <c r="D31" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="E31" t="e">
-        <f>ACOS(C31)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>1</v>
-      </c>
-      <c r="B33">
-        <f>ACOS(A33)</f>
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <f>A33-0.1</f>
-        <v>0.9</v>
-      </c>
-      <c r="B34">
-        <f t="shared" ref="B34:B42" si="7">ACOS(A34)</f>
-        <v>0.45102681179626236</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <f>A34-0.1</f>
-        <v>0.8</v>
-      </c>
-      <c r="B35">
-        <f t="shared" si="7"/>
-        <v>0.64350110879328426</v>
-      </c>
-      <c r="C35">
-        <f>PI()/4</f>
-        <v>0.78539816339744828</v>
-      </c>
-      <c r="D35" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <f>A35-0.1</f>
-        <v>0.70000000000000007</v>
-      </c>
-      <c r="B36">
-        <f t="shared" si="7"/>
-        <v>0.79539883018414337</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <f>A36-0.1</f>
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="B37">
-        <f t="shared" si="7"/>
-        <v>0.92729521800161208</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <f t="shared" ref="A38:A42" si="8">A37-0.1</f>
-        <v>0.50000000000000011</v>
-      </c>
-      <c r="B38">
-        <f t="shared" si="7"/>
-        <v>1.0471975511965974</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <f t="shared" si="8"/>
-        <v>0.40000000000000013</v>
-      </c>
-      <c r="B39">
-        <f t="shared" si="7"/>
-        <v>1.1592794807274083</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <f t="shared" si="8"/>
-        <v>0.30000000000000016</v>
-      </c>
-      <c r="B40">
-        <f t="shared" si="7"/>
-        <v>1.266103672779499</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <f t="shared" si="8"/>
-        <v>0.20000000000000015</v>
-      </c>
-      <c r="B41">
-        <f t="shared" si="7"/>
-        <v>1.3694384060045657</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <f t="shared" si="8"/>
-        <v>0.10000000000000014</v>
-      </c>
-      <c r="B42">
-        <f t="shared" si="7"/>
-        <v>1.4706289056333366</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>0</v>
-      </c>
-      <c r="B43">
-        <f>ACOS(A43)</f>
-        <v>1.5707963267948966</v>
-      </c>
-      <c r="C43">
-        <f>PI()/2</f>
-        <v>1.5707963267948966</v>
-      </c>
-      <c r="D43" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <f>A43-0.1</f>
-        <v>-0.1</v>
-      </c>
-      <c r="B44">
-        <f>ACOS(A44)</f>
-        <v>1.6709637479564563</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <f>A44-0.1</f>
-        <v>-0.2</v>
-      </c>
-      <c r="B45">
-        <f>ACOS(A45)</f>
-        <v>1.7721542475852274</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <f t="shared" ref="A46:A64" si="9">A45-0.1</f>
-        <v>-0.30000000000000004</v>
-      </c>
-      <c r="B46">
-        <f t="shared" ref="B46:B66" si="10">ACOS(A46)</f>
-        <v>1.8754889808102941</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <f t="shared" si="9"/>
-        <v>-0.4</v>
-      </c>
-      <c r="B47">
-        <f t="shared" si="10"/>
-        <v>1.9823131728623846</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <f t="shared" si="9"/>
-        <v>-0.5</v>
-      </c>
-      <c r="B48">
-        <f t="shared" si="10"/>
-        <v>2.0943951023931957</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <f t="shared" si="9"/>
-        <v>-0.6</v>
-      </c>
-      <c r="B49">
-        <f t="shared" si="10"/>
-        <v>2.2142974355881808</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <f t="shared" si="9"/>
-        <v>-0.7</v>
-      </c>
-      <c r="B50">
-        <f t="shared" si="10"/>
-        <v>2.3461938234056499</v>
-      </c>
-      <c r="C50">
-        <f>(3/4)*PI()</f>
-        <v>2.3561944901923448</v>
-      </c>
-      <c r="D50" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <f t="shared" si="9"/>
-        <v>-0.79999999999999993</v>
-      </c>
-      <c r="B51">
-        <f t="shared" si="10"/>
-        <v>2.4980915447965089</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <f t="shared" si="9"/>
-        <v>-0.89999999999999991</v>
-      </c>
-      <c r="B52">
-        <f t="shared" si="10"/>
-        <v>2.6905658417935303</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <f t="shared" si="9"/>
-        <v>-0.99999999999999989</v>
-      </c>
-      <c r="B53">
-        <f t="shared" si="10"/>
-        <v>3.1415926535897931</v>
-      </c>
-      <c r="C53">
-        <f>PI()</f>
-        <v>3.1415926535897931</v>
-      </c>
-      <c r="D53" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54">
-        <f t="shared" si="9"/>
-        <v>-1.0999999999999999</v>
-      </c>
-      <c r="B54" t="e">
-        <f t="shared" si="10"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55">
-        <f t="shared" si="9"/>
-        <v>-1.2</v>
-      </c>
-      <c r="B55" t="e">
-        <f t="shared" si="10"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56">
-        <f t="shared" si="9"/>
-        <v>-1.3</v>
-      </c>
-      <c r="B56" t="e">
-        <f t="shared" si="10"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57">
-        <f t="shared" si="9"/>
-        <v>-1.4000000000000001</v>
-      </c>
-      <c r="B57" t="e">
-        <f t="shared" si="10"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58">
-        <f t="shared" si="9"/>
-        <v>-1.5000000000000002</v>
-      </c>
-      <c r="B58" t="e">
-        <f t="shared" si="10"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59">
-        <f t="shared" si="9"/>
-        <v>-1.6000000000000003</v>
-      </c>
-      <c r="B59" t="e">
-        <f t="shared" si="10"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60">
-        <f t="shared" si="9"/>
-        <v>-1.7000000000000004</v>
-      </c>
-      <c r="B60" t="e">
-        <f t="shared" si="10"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61">
-        <f t="shared" si="9"/>
-        <v>-1.8000000000000005</v>
-      </c>
-      <c r="B61" t="e">
-        <f t="shared" si="10"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62">
-        <f t="shared" si="9"/>
-        <v>-1.9000000000000006</v>
-      </c>
-      <c r="B62" t="e">
-        <f t="shared" si="10"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63">
-        <f t="shared" si="9"/>
-        <v>-2.0000000000000004</v>
-      </c>
-      <c r="B63" t="e">
-        <f t="shared" si="10"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64">
-        <f t="shared" si="9"/>
-        <v>-2.1000000000000005</v>
-      </c>
-      <c r="B64" t="e">
-        <f t="shared" si="10"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65">
-        <f>A64-0.1</f>
-        <v>-2.2000000000000006</v>
-      </c>
-      <c r="B65" t="e">
-        <f>ACOS(A65)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66">
-        <f t="shared" ref="A66" si="11">A65-0.1</f>
-        <v>-2.3000000000000007</v>
-      </c>
-      <c r="B66" t="e">
-        <f t="shared" si="10"/>
-        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>
@@ -9688,13 +9218,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{980E11E1-220A-447B-A3F4-1C24A01EFBA2}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
@@ -10282,7 +9818,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2</v>
       </c>
@@ -10301,7 +9837,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2</v>
       </c>
@@ -10318,6 +9854,540 @@
       <c r="E34">
         <f t="shared" si="7"/>
         <v>-1.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>3</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <f>A38*COS(C38)-B38*SIN(C38)</f>
+        <v>3</v>
+      </c>
+      <c r="E38">
+        <f>A38*SIN(C38)+B38*COS(C38)</f>
+        <v>4</v>
+      </c>
+      <c r="G38" t="str">
+        <f>"[TestCase("&amp;A38&amp;","&amp;B38&amp;","&amp;ROUND(C38,6)&amp;","&amp;ROUND(D38,6)&amp;","&amp;ROUND(E38,6)&amp;")]"</f>
+        <v>[TestCase(3,4,0,3,4)]</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <f>PI()/4</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="D39">
+        <f>A39*COS(C39)-B39*SIN(C39)</f>
+        <v>-0.70710678118654702</v>
+      </c>
+      <c r="E39">
+        <f t="shared" ref="E39:E46" si="8">A39*SIN(C39)+B39*COS(C39)</f>
+        <v>4.9497474683058327</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" ref="G39:G46" si="9">"[TestCase("&amp;A39&amp;","&amp;B39&amp;","&amp;ROUND(C39,6)&amp;","&amp;ROUND(D39,6)&amp;","&amp;ROUND(E39,6)&amp;")]"</f>
+        <v>[TestCase(3,4,0.785398,-0.707107,4.949747)]</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40">
+        <f>PI()/2</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="D40">
+        <f t="shared" ref="D39:D46" si="10">A40*COS(C40)-B40*SIN(C40)</f>
+        <v>-4</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="8"/>
+        <v>3.0000000000000004</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="9"/>
+        <v>[TestCase(3,4,1.570796,-4,3)]</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>3</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41">
+        <f>(3/4)*PI()</f>
+        <v>2.3561944901923448</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="10"/>
+        <v>-4.9497474683058327</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="8"/>
+        <v>-0.70710678118654702</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="9"/>
+        <v>[TestCase(3,4,2.356194,-4.949747,-0.707107)]</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>3</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="10"/>
+        <v>-3.0000000000000004</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="8"/>
+        <v>-3.9999999999999996</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="9"/>
+        <v>[TestCase(3,4,3.141593,-3,-4)]</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43">
+        <f>(5/4)*PI()</f>
+        <v>3.9269908169872414</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="10"/>
+        <v>0.70710678118654702</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="8"/>
+        <v>-4.9497474683058336</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="9"/>
+        <v>[TestCase(3,4,3.926991,0.707107,-4.949747)]</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>3</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44">
+        <f>(3/2)*PI()</f>
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="10"/>
+        <v>3.9999999999999996</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="8"/>
+        <v>-3.0000000000000009</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="9"/>
+        <v>[TestCase(3,4,4.712389,4,-3)]</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <f>(7/4)*PI()</f>
+        <v>5.497787143782138</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="10"/>
+        <v>4.9497474683058327</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="8"/>
+        <v>0.70710678118654657</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="9"/>
+        <v>[TestCase(3,4,5.497787,4.949747,0.707107)]</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>3</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46">
+        <f>2*PI()</f>
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="10"/>
+        <v>3.0000000000000009</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="8"/>
+        <v>3.9999999999999991</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="9"/>
+        <v>[TestCase(3,4,6.283185,3,4)]</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <f>((A50-C50)*COS(E50)-(B50-D50)*SIN(E50))+C50</f>
+        <v>3</v>
+      </c>
+      <c r="G50">
+        <f>((A50-C50)*SIN(E50)+(B50-D50)*COS(E50))+D50</f>
+        <v>4</v>
+      </c>
+      <c r="I50" t="str">
+        <f>"[TestCase("&amp;A50&amp;","&amp;B50&amp;","&amp;C50&amp;","&amp;D50&amp;","&amp;ROUND(E50,6)&amp;","&amp;ROUND(F50,6)&amp;","&amp;ROUND(G50,6)&amp;")]"</f>
+        <v>[TestCase(3,4,2,1,0,3,4)]</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <f>PI()/4</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="F51">
+        <f t="shared" ref="F51:F58" si="11">((A51-C51)*COS(E51)-(B51-D51)*SIN(E51))+C51</f>
+        <v>0.58578643762690508</v>
+      </c>
+      <c r="G51">
+        <f t="shared" ref="G51:G58" si="12">((A51-C51)*SIN(E51)+(B51-D51)*COS(E51))+D51</f>
+        <v>3.8284271247461903</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" ref="I51:I58" si="13">"[TestCase("&amp;A51&amp;","&amp;B51&amp;","&amp;C51&amp;","&amp;D51&amp;","&amp;ROUND(E51,6)&amp;","&amp;ROUND(F51,6)&amp;","&amp;ROUND(G51,6)&amp;")]"</f>
+        <v>[TestCase(3,4,2,1,0.785398,0.585786,3.828427)]</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>3</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <f>PI()/2</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="11"/>
+        <v>-1</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="I52" t="str">
+        <f t="shared" si="13"/>
+        <v>[TestCase(3,4,2,1,1.570796,-1,2)]</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>3</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <f>(3/4)*PI()</f>
+        <v>2.3561944901923448</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="11"/>
+        <v>-0.82842712474619029</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="12"/>
+        <v>-0.41421356237309492</v>
+      </c>
+      <c r="I53" t="str">
+        <f t="shared" si="13"/>
+        <v>[TestCase(3,4,2,1,2.356194,-0.828427,-0.414214)]</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>3</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="11"/>
+        <v>0.99999999999999956</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="12"/>
+        <v>-2</v>
+      </c>
+      <c r="I54" t="str">
+        <f t="shared" si="13"/>
+        <v>[TestCase(3,4,2,1,3.141593,1,-2)]</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>3</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <f>(5/4)*PI()</f>
+        <v>3.9269908169872414</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="11"/>
+        <v>3.4142135623730949</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="12"/>
+        <v>-1.8284271247461903</v>
+      </c>
+      <c r="I55" t="str">
+        <f t="shared" si="13"/>
+        <v>[TestCase(3,4,2,1,3.926991,3.414214,-1.828427)]</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>3</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <f>(3/2)*PI()</f>
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="I56" t="str">
+        <f t="shared" si="13"/>
+        <v>[TestCase(3,4,2,1,4.712389,5,0)]</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>3</v>
+      </c>
+      <c r="B57">
+        <v>4</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <f>(7/4)*PI()</f>
+        <v>5.497787143782138</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="11"/>
+        <v>4.8284271247461898</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="12"/>
+        <v>2.414213562373094</v>
+      </c>
+      <c r="I57" t="str">
+        <f t="shared" si="13"/>
+        <v>[TestCase(3,4,2,1,5.497787,4.828427,2.414214)]</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>3</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <f>2*PI()</f>
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="11"/>
+        <v>3.0000000000000009</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="12"/>
+        <v>3.9999999999999996</v>
+      </c>
+      <c r="I58" t="str">
+        <f t="shared" si="13"/>
+        <v>[TestCase(3,4,2,1,6.283185,3,4)]</v>
       </c>
     </row>
   </sheetData>
@@ -13805,8 +13875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A61F9444-A8E7-4D49-9ABE-CE6471863689}">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92:XFD102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added Polar Coordinate Tests
Including minor fixes due to failing tests.
</commit_message>
<xml_diff>
--- a/docs/Math Tests.xlsx
+++ b/docs/Math Tests.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\personal\MPT.Net\MPT\Math\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F13126A-F0F9-4937-815A-5ED16E28F82A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453D9F6D-33C4-4F8A-AB74-006FA8610F04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="824" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="824" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Numbers" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <sheet name="CartesianOffsets" sheetId="8" r:id="rId8"/>
     <sheet name="Angle" sheetId="7" r:id="rId9"/>
     <sheet name="AngleOffsets" sheetId="9" r:id="rId10"/>
-    <sheet name="Vectors" sheetId="10" r:id="rId11"/>
+    <sheet name="PolarCoordinate" sheetId="12" r:id="rId11"/>
+    <sheet name="PolarOffset" sheetId="13" r:id="rId12"/>
+    <sheet name="Vectors" sheetId="10" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="a_2" localSheetId="1">Algebra!$C$307</definedName>
@@ -59,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="205">
   <si>
     <t>Cube Root</t>
   </si>
@@ -608,6 +610,72 @@
   </si>
   <si>
     <t>Ycenter</t>
+  </si>
+  <si>
+    <t>SubtractAngleAzimuthRadians_Returns_Difference_Between_Angles</t>
+  </si>
+  <si>
+    <t>angle 1</t>
+  </si>
+  <si>
+    <t>angle 2</t>
+  </si>
+  <si>
+    <t>AddAngleAzimuthDegrees_Returns_Combined_Angles</t>
+  </si>
+  <si>
+    <t>SubtractOverride_Subtracting_Coordinate_Returns_Coordinate_Offset_Between_Coordinates</t>
+  </si>
+  <si>
+    <t>angle</t>
+  </si>
+  <si>
+    <t>radiusI2</t>
+  </si>
+  <si>
+    <t>angleI2</t>
+  </si>
+  <si>
+    <t>radiusJ2</t>
+  </si>
+  <si>
+    <t>angleJ2</t>
+  </si>
+  <si>
+    <t>radiusResult</t>
+  </si>
+  <si>
+    <t>angleResult</t>
+  </si>
+  <si>
+    <t>offset-coordinate</t>
+  </si>
+  <si>
+    <t>coordinate-offset</t>
+  </si>
+  <si>
+    <t>offset+coordinate</t>
+  </si>
+  <si>
+    <t>coordinate+offset</t>
+  </si>
+  <si>
+    <t>Length_Returns_Linear_Distance_Between_Offset_Points</t>
+  </si>
+  <si>
+    <t>radiusI</t>
+  </si>
+  <si>
+    <t>angleI</t>
+  </si>
+  <si>
+    <t>radiusJ</t>
+  </si>
+  <si>
+    <t>angleJ</t>
+  </si>
+  <si>
+    <t>distance</t>
   </si>
 </sst>
 </file>
@@ -719,7 +787,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -767,6 +835,9 @@
     <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1048,6 +1119,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E817D384-0C7C-40C4-9B8C-466473A6AF3F}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1256,6 +1328,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2398FD5B-93B3-4E50-9380-18A3BF1F0024}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1540,7 +1613,1159 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98CE41AE-4B4C-45FB-B105-D99E7FB8D10E}">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="B3">
+        <f>PI()/4</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="C3">
+        <f>A3-B3</f>
+        <v>2.3561944901923448</v>
+      </c>
+      <c r="D3">
+        <f>(3/4)*PI()</f>
+        <v>2.3561944901923448</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="B4">
+        <f>-PI()/4</f>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C13" si="0">A4-B4</f>
+        <v>3.9269908169872414</v>
+      </c>
+      <c r="D4">
+        <f>(5/4)*PI()</f>
+        <v>3.9269908169872414</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f>-PI()</f>
+        <v>-3.1415926535897931</v>
+      </c>
+      <c r="B5">
+        <f>PI()/4</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>-3.9269908169872414</v>
+      </c>
+      <c r="D5">
+        <f>-(5/4)*PI()</f>
+        <v>-3.9269908169872414</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f>-PI()</f>
+        <v>-3.1415926535897931</v>
+      </c>
+      <c r="B6">
+        <f>-PI()/4</f>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>-2.3561944901923448</v>
+      </c>
+      <c r="D6">
+        <f>-(3/4)*PI()</f>
+        <v>-2.3561944901923448</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>45</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>45</v>
+      </c>
+      <c r="B9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>42.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>45</v>
+      </c>
+      <c r="B10">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>47.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>-45</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>-49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>-45</v>
+      </c>
+      <c r="B12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>-47.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>-45</v>
+      </c>
+      <c r="B13">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>-42.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>45</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <f>A16+B16</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>45</v>
+      </c>
+      <c r="B17">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:C21" si="1">A17+B17</f>
+        <v>47.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>45</v>
+      </c>
+      <c r="B18">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>42.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>-45</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>-41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>-45</v>
+      </c>
+      <c r="B20">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>-42.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>-45</v>
+      </c>
+      <c r="B21">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>-47.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE412607-CC50-46B5-B624-B25F930CD5D9}">
+  <dimension ref="A1:N24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18:G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41" t="s">
+        <v>197</v>
+      </c>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41" t="s">
+        <v>198</v>
+      </c>
+      <c r="N2" s="41"/>
+    </row>
+    <row r="3" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f>(E4-C4)-A4</f>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f>(F4-D4)-B4</f>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f>A4-(E4-C4)</f>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f>B4-(F4-D4)</f>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f>(E4-C4)+A4</f>
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f>(F4-D4)+B4</f>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f>A4+(E4-C4)</f>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f>B4+(F4-D4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <f>PI()/4</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <f>PI()/2</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="G5">
+        <f>(E5-C5)-A5</f>
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <f>(F5-D5)-B5</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="I5">
+        <f>A5-(E5-C5)</f>
+        <v>-1</v>
+      </c>
+      <c r="J5">
+        <f>B5-(F5-D5)</f>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:K14" si="0">(E5-C5)+A5</f>
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:L14" si="1">(F5-D5)+B5</f>
+        <v>2.3561944901923448</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M14" si="2">A5+(E5-C5)</f>
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ref="N5:N14" si="3">B5+(F5-D5)</f>
+        <v>2.3561944901923448</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>-1</v>
+      </c>
+      <c r="B6">
+        <f>PI()/4</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="C6">
+        <v>-5</v>
+      </c>
+      <c r="D6">
+        <f>PI()/2</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="E6">
+        <v>-7</v>
+      </c>
+      <c r="F6">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" ref="G6:G14" si="4">(E6-C6)-A6</f>
+        <v>-1</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" ref="H6:H14" si="5">(F6-D6)-B6</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" ref="I6:I14" si="6">A6-(E6-C6)</f>
+        <v>1</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" ref="J6:J14" si="7">B6-(F6-D6)</f>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>2.3561944901923448</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="3"/>
+        <v>2.3561944901923448</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>-1</v>
+      </c>
+      <c r="B7" s="30">
+        <f>-PI()/4</f>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="C7">
+        <v>-5</v>
+      </c>
+      <c r="D7" s="30">
+        <f>-PI()/2</f>
+        <v>-1.5707963267948966</v>
+      </c>
+      <c r="E7">
+        <v>-7</v>
+      </c>
+      <c r="F7" s="30">
+        <f>-PI()</f>
+        <v>-3.1415926535897931</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="5"/>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="7"/>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>-2.3561944901923448</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="3"/>
+        <v>-2.3561944901923448</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="30">
+        <f>-PI()/4</f>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8" s="30">
+        <f t="shared" ref="D8:D9" si="8">-PI()/2</f>
+        <v>-1.5707963267948966</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8" s="30">
+        <f>-PI()</f>
+        <v>-3.1415926535897931</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="5"/>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="7"/>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>-2.3561944901923448</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="3"/>
+        <v>-2.3561944901923448</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ref="B9:B14" si="9">PI()/4</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="C9">
+        <v>-5</v>
+      </c>
+      <c r="D9" s="30">
+        <f t="shared" si="8"/>
+        <v>-1.5707963267948966</v>
+      </c>
+      <c r="E9">
+        <v>-7</v>
+      </c>
+      <c r="F9" s="30">
+        <f>-PI()</f>
+        <v>-3.1415926535897931</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="4"/>
+        <v>-3</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="5"/>
+        <v>-2.3561944901923448</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="7"/>
+        <v>2.3561944901923448</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="3"/>
+        <v>-0.78539816339744828</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="9"/>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="C10">
+        <v>-5</v>
+      </c>
+      <c r="D10">
+        <f>PI()/2</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="E10">
+        <v>-7</v>
+      </c>
+      <c r="F10">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="4"/>
+        <v>-3</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="5"/>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="7"/>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>2.3561944901923448</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="3"/>
+        <v>2.3561944901923448</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="9"/>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11" s="30">
+        <f>-PI()/2</f>
+        <v>-1.5707963267948966</v>
+      </c>
+      <c r="E11">
+        <v>7</v>
+      </c>
+      <c r="F11" s="30">
+        <f>-PI()</f>
+        <v>-3.1415926535897931</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="5"/>
+        <v>-2.3561944901923448</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="7"/>
+        <v>2.3561944901923448</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="3"/>
+        <v>-0.78539816339744828</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="9"/>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ref="D12:D14" si="10">PI()/2</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="5"/>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="7"/>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>2.3561944901923448</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="3"/>
+        <v>2.3561944901923448</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="9"/>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="10"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="5"/>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="7"/>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>2.3561944901923448</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="3"/>
+        <v>2.3561944901923448</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="9"/>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="C14">
+        <v>5.5</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="10"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="E14">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F14">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="4"/>
+        <v>-2.1999999999999997</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="5"/>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="6"/>
+        <v>2.1999999999999997</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="7"/>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>2.3561944901923448</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="3"/>
+        <v>2.3561944901923448</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f>SQRT(A18^2+C18^2-2*A18*C18*COS(D18-B18))</f>
+        <v>0</v>
+      </c>
+      <c r="G18" t="str">
+        <f>"[TestCase("&amp;A18&amp;", "&amp;ROUND(B18,6)&amp;", "&amp;C18&amp;", "&amp;ROUND(D18,6)&amp;", "&amp;ROUND(E18,6)&amp;")]"</f>
+        <v>[TestCase(0, 0, 0, 0, 0)]</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ref="E19:E24" si="11">SQRT(A19^2+C19^2-2*A19*C19*COS(D19-B19))</f>
+        <v>0</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" ref="G19:G24" si="12">"[TestCase("&amp;A19&amp;", "&amp;ROUND(B19,6)&amp;", "&amp;C19&amp;", "&amp;ROUND(D19,6)&amp;", "&amp;ROUND(E19,6)&amp;")]"</f>
+        <v>[TestCase(0, 0, 0, 1, 0)]</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="12"/>
+        <v>[TestCase(0, 0, 1, 0, 1)]</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B21">
+        <f>PI()/4</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="C21">
+        <v>3.3</v>
+      </c>
+      <c r="D21">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="11"/>
+        <v>4.1513365596412841</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="12"/>
+        <v>[TestCase(1.1, 0.785398, 3.3, 3.141593, 4.151337)]</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B22">
+        <f>-PI()/4</f>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="C22">
+        <v>-3.3</v>
+      </c>
+      <c r="D22">
+        <f>-PI()</f>
+        <v>-3.1415926535897931</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="11"/>
+        <v>2.6393947731602534</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="12"/>
+        <v>[TestCase(1.1, -0.785398, -3.3, -3.141593, 2.639395)]</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="B23">
+        <f>-PI()/4</f>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="C23">
+        <v>-3.3</v>
+      </c>
+      <c r="D23">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="11"/>
+        <v>4.1513365596412841</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="12"/>
+        <v>[TestCase(-1.1, -0.785398, -3.3, 3.141593, 4.151337)]</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="B24">
+        <f>-PI()/4</f>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="C24">
+        <v>3.3</v>
+      </c>
+      <c r="D24">
+        <f>-PI()</f>
+        <v>-3.1415926535897931</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="11"/>
+        <v>2.6393947731602534</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="12"/>
+        <v>[TestCase(-1.1, -0.785398, 3.3, -3.141593, 2.639395)]</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78894319-A7BE-40F1-B4B5-401399411CE5}">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
@@ -2342,6 +3567,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -3180,6 +4406,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67CCEAE-A218-4C94-819E-031E3B1F04E0}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3194,6 +4421,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8705911-FCC4-4561-9B15-FA5562CD2EAD}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -4954,6 +6182,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4692FF0-D374-4E44-BAFE-C6C855E4487F}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4978,6 +6207,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7EB2C40-5C39-4337-BA16-2FE8050D6AEB}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:P125"/>
   <sheetViews>
     <sheetView topLeftCell="A100" workbookViewId="0">
@@ -9218,9 +10448,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{980E11E1-220A-447B-A3F4-1C24A01EFBA2}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
@@ -10398,10 +11629,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57857484-DE77-4489-8505-7605FEA3DB06}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:O114"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38:L48"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="L83" sqref="L83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13873,10 +15105,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A61F9444-A8E7-4D49-9ABE-CE6471863689}">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:G121"/>
   <sheetViews>
     <sheetView topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92:XFD102"/>
+      <selection activeCell="I106" sqref="I106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Unit Testing Algebra Library
Got to 100% coverage.
</commit_message>
<xml_diff>
--- a/docs/Math Tests.xlsx
+++ b/docs/Math Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\personal\MPT.Net\MPT\Math\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453D9F6D-33C4-4F8A-AB74-006FA8610F04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D099A7F9-C892-4110-91D2-48D50C25ACEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="824" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="242">
   <si>
     <t>Cube Root</t>
   </si>
@@ -676,6 +676,117 @@
   </si>
   <si>
     <t>distance</t>
+  </si>
+  <si>
+    <t>InterpolationLinear2D</t>
+  </si>
+  <si>
+    <t>Wii</t>
+  </si>
+  <si>
+    <t>Wij</t>
+  </si>
+  <si>
+    <t>Wji</t>
+  </si>
+  <si>
+    <t>Wjj</t>
+  </si>
+  <si>
+    <t>row i</t>
+  </si>
+  <si>
+    <t>row j</t>
+  </si>
+  <si>
+    <t>col i</t>
+  </si>
+  <si>
+    <t>col j</t>
+  </si>
+  <si>
+    <t>value ii</t>
+  </si>
+  <si>
+    <t>value jj</t>
+  </si>
+  <si>
+    <t>value ij</t>
+  </si>
+  <si>
+    <t>value ji</t>
+  </si>
+  <si>
+    <t>col 0</t>
+  </si>
+  <si>
+    <t>row 0</t>
+  </si>
+  <si>
+    <t>All Corners have same value</t>
+  </si>
+  <si>
+    <t>Top Edge</t>
+  </si>
+  <si>
+    <t>Left Edge</t>
+  </si>
+  <si>
+    <t>Right Edge</t>
+  </si>
+  <si>
+    <t>Pt ii</t>
+  </si>
+  <si>
+    <t>Pt jj</t>
+  </si>
+  <si>
+    <t>Pt ij</t>
+  </si>
+  <si>
+    <t>Pt ji</t>
+  </si>
+  <si>
+    <t>Center of plane sloped along rows</t>
+  </si>
+  <si>
+    <t>Center of plane sloped along columns</t>
+  </si>
+  <si>
+    <t>All corners have different value, point not centered</t>
+  </si>
+  <si>
+    <t>Bottom Edge</t>
+  </si>
+  <si>
+    <t>Width of 0</t>
+  </si>
+  <si>
+    <t>Heigh of 0</t>
+  </si>
+  <si>
+    <t>IntersectionX</t>
+  </si>
+  <si>
+    <t>vertical line</t>
+  </si>
+  <si>
+    <t>within points</t>
+  </si>
+  <si>
+    <t>outside of points</t>
+  </si>
+  <si>
+    <t>points are equal</t>
+  </si>
+  <si>
+    <t>negative slope</t>
+  </si>
+  <si>
+    <t>parallel</t>
+  </si>
+  <si>
+    <t>collinear</t>
   </si>
 </sst>
 </file>
@@ -787,7 +898,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -838,6 +949,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1866,10 +1980,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE412607-CC50-46B5-B624-B25F930CD5D9}">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:T52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18:G24"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2571,7 +2685,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>200</v>
       </c>
@@ -2588,7 +2702,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
@@ -2610,7 +2724,7 @@
         <v>[TestCase(0, 0, 0, 0, 0)]</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0</v>
       </c>
@@ -2632,7 +2746,7 @@
         <v>[TestCase(0, 0, 0, 1, 0)]</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0</v>
       </c>
@@ -2654,7 +2768,7 @@
         <v>[TestCase(0, 0, 1, 0, 1)]</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1.1000000000000001</v>
       </c>
@@ -2678,7 +2792,7 @@
         <v>[TestCase(1.1, 0.785398, 3.3, 3.141593, 4.151337)]</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1.1000000000000001</v>
       </c>
@@ -2702,7 +2816,7 @@
         <v>[TestCase(1.1, -0.785398, -3.3, -3.141593, 2.639395)]</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>-1.1000000000000001</v>
       </c>
@@ -2726,7 +2840,7 @@
         <v>[TestCase(-1.1, -0.785398, -3.3, 3.141593, 4.151337)]</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>-1.1000000000000001</v>
       </c>
@@ -2748,6 +2862,1220 @@
       <c r="G24" t="str">
         <f t="shared" si="12"/>
         <v>[TestCase(-1.1, -0.785398, 3.3, -3.141593, 2.639395)]</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="J27" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="M27" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="N27" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="O27" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="P27" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A28" s="42">
+        <v>0</v>
+      </c>
+      <c r="B28" s="43">
+        <v>0</v>
+      </c>
+      <c r="C28" s="10">
+        <v>0</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0</v>
+      </c>
+      <c r="E28" s="42">
+        <v>0</v>
+      </c>
+      <c r="F28" s="43">
+        <v>0</v>
+      </c>
+      <c r="G28" s="42">
+        <v>0</v>
+      </c>
+      <c r="H28" s="44">
+        <v>0</v>
+      </c>
+      <c r="I28" s="44">
+        <v>0</v>
+      </c>
+      <c r="J28" s="43">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <f>(A28-C28)*(B28-D28)</f>
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f>(E28-A28)*(B28-D28)</f>
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f>(A28-C28)*(F28-B28)</f>
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <f>(E28-A28)*(F28-B28)</f>
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <f>(E28-C28)*(F28-D28)</f>
+        <v>0</v>
+      </c>
+      <c r="P28" t="e">
+        <f>(G28*N28+H28*M28+I28*L28+J28*K28)/O28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T28" t="e">
+        <f>"[TestCase("&amp;A28&amp;", "&amp;B28&amp;", "&amp;C28&amp;", "&amp;D28&amp;", "&amp;E28&amp;", "&amp;F28&amp;", "&amp;G28&amp;", "&amp;H28&amp;", "&amp;I28&amp;", "&amp;J28&amp;", "&amp;ROUND(P28,6)&amp;")]  // " &amp;Q28</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A29" s="42">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B29" s="43">
+        <v>3.3</v>
+      </c>
+      <c r="C29" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D29" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E29" s="42">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F29" s="43">
+        <v>6.6</v>
+      </c>
+      <c r="G29" s="42">
+        <v>1.5</v>
+      </c>
+      <c r="H29" s="44">
+        <v>1.5</v>
+      </c>
+      <c r="I29" s="44">
+        <v>1.5</v>
+      </c>
+      <c r="J29" s="43">
+        <v>1.5</v>
+      </c>
+      <c r="K29">
+        <f>(A29-C29)*(B29-D29)</f>
+        <v>1.2099999999999997</v>
+      </c>
+      <c r="L29">
+        <f>(E29-A29)*(B29-D29)</f>
+        <v>-1.2099999999999997</v>
+      </c>
+      <c r="M29">
+        <f>(A29-C29)*(F29-B29)</f>
+        <v>3.63</v>
+      </c>
+      <c r="N29">
+        <f>(E29-A29)*(F29-B29)</f>
+        <v>-3.63</v>
+      </c>
+      <c r="O29">
+        <f>(E29-C29)*(F29-D29)</f>
+        <v>0</v>
+      </c>
+      <c r="P29" t="e">
+        <f>(G29*N29+H29*M29+I29*L29+J29*K29)/O29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>232</v>
+      </c>
+      <c r="T29" t="e">
+        <f t="shared" ref="T29:T42" si="13">"[TestCase("&amp;A29&amp;", "&amp;B29&amp;", "&amp;C29&amp;", "&amp;D29&amp;", "&amp;E29&amp;", "&amp;F29&amp;", "&amp;G29&amp;", "&amp;H29&amp;", "&amp;I29&amp;", "&amp;J29&amp;", "&amp;ROUND(P29,6)&amp;")]  // " &amp;Q29</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A30" s="42">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B30" s="43">
+        <v>3.3</v>
+      </c>
+      <c r="C30" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D30" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E30" s="42">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F30" s="43">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G30" s="42">
+        <v>1.5</v>
+      </c>
+      <c r="H30" s="44">
+        <v>1.5</v>
+      </c>
+      <c r="I30" s="44">
+        <v>1.5</v>
+      </c>
+      <c r="J30" s="43">
+        <v>1.5</v>
+      </c>
+      <c r="K30">
+        <f>(A30-C30)*(B30-D30)</f>
+        <v>1.2099999999999997</v>
+      </c>
+      <c r="L30">
+        <f>(E30-A30)*(B30-D30)</f>
+        <v>2.4199999999999995</v>
+      </c>
+      <c r="M30">
+        <f>(A30-C30)*(F30-B30)</f>
+        <v>-1.2099999999999997</v>
+      </c>
+      <c r="N30">
+        <f>(E30-A30)*(F30-B30)</f>
+        <v>-2.4199999999999995</v>
+      </c>
+      <c r="O30">
+        <f>(E30-C30)*(F30-D30)</f>
+        <v>0</v>
+      </c>
+      <c r="P30" t="e">
+        <f>(G30*N30+H30*M30+I30*L30+J30*K30)/O30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>233</v>
+      </c>
+      <c r="T30" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A31" s="42">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B31" s="43">
+        <v>3.3</v>
+      </c>
+      <c r="C31" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D31" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E31" s="42">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F31" s="43">
+        <v>6.6</v>
+      </c>
+      <c r="G31" s="42">
+        <v>1.5</v>
+      </c>
+      <c r="H31" s="44">
+        <v>1.5</v>
+      </c>
+      <c r="I31" s="44">
+        <v>1.5</v>
+      </c>
+      <c r="J31" s="43">
+        <v>1.5</v>
+      </c>
+      <c r="K31">
+        <f>(A31-C31)*(B31-D31)</f>
+        <v>1.2099999999999997</v>
+      </c>
+      <c r="L31">
+        <f>(E31-A31)*(B31-D31)</f>
+        <v>2.4199999999999995</v>
+      </c>
+      <c r="M31">
+        <f>(A31-C31)*(F31-B31)</f>
+        <v>3.63</v>
+      </c>
+      <c r="N31">
+        <f>(E31-A31)*(F31-B31)</f>
+        <v>7.26</v>
+      </c>
+      <c r="O31">
+        <f>(E31-C31)*(F31-D31)</f>
+        <v>14.52</v>
+      </c>
+      <c r="P31">
+        <f>(G31*N31+H31*M31+I31*L31+J31*K31)/O31</f>
+        <v>1.5000000000000002</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>220</v>
+      </c>
+      <c r="T31" t="str">
+        <f t="shared" si="13"/>
+        <v>[TestCase(2.2, 3.3, 1.1, 2.2, 4.4, 6.6, 1.5, 1.5, 1.5, 1.5, 1.5)]  // All Corners have same value</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A32" s="42">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B32" s="43">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C32" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D32" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E32" s="42">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F32" s="43">
+        <v>6.6</v>
+      </c>
+      <c r="G32" s="42">
+        <v>1</v>
+      </c>
+      <c r="H32" s="44">
+        <v>2</v>
+      </c>
+      <c r="I32" s="44">
+        <v>3</v>
+      </c>
+      <c r="J32" s="43">
+        <v>4</v>
+      </c>
+      <c r="K32">
+        <f>(A32-C32)*(B32-D32)</f>
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <f>(E32-A32)*(B32-D32)</f>
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <f>(A32-C32)*(F32-B32)</f>
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <f>(E32-A32)*(F32-B32)</f>
+        <v>14.52</v>
+      </c>
+      <c r="O32">
+        <f>(E32-C32)*(F32-D32)</f>
+        <v>14.52</v>
+      </c>
+      <c r="P32">
+        <f>(G32*N32+H32*M32+I32*L32+J32*K32)/O32</f>
+        <v>1</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>224</v>
+      </c>
+      <c r="T32" t="str">
+        <f t="shared" si="13"/>
+        <v>[TestCase(1.1, 2.2, 1.1, 2.2, 4.4, 6.6, 1, 2, 3, 4, 1)]  // Pt ii</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A33" s="42">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B33" s="43">
+        <v>6.6</v>
+      </c>
+      <c r="C33" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D33" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E33" s="42">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F33" s="43">
+        <v>6.6</v>
+      </c>
+      <c r="G33" s="42">
+        <v>1</v>
+      </c>
+      <c r="H33" s="44">
+        <v>2</v>
+      </c>
+      <c r="I33" s="44">
+        <v>3</v>
+      </c>
+      <c r="J33" s="43">
+        <v>4</v>
+      </c>
+      <c r="K33">
+        <f>(A33-C33)*(B33-D33)</f>
+        <v>14.52</v>
+      </c>
+      <c r="L33">
+        <f>(E33-A33)*(B33-D33)</f>
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <f>(A33-C33)*(F33-B33)</f>
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <f>(E33-A33)*(F33-B33)</f>
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <f>(E33-C33)*(F33-D33)</f>
+        <v>14.52</v>
+      </c>
+      <c r="P33">
+        <f>(G33*N33+H33*M33+I33*L33+J33*K33)/O33</f>
+        <v>4</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>225</v>
+      </c>
+      <c r="T33" t="str">
+        <f t="shared" si="13"/>
+        <v>[TestCase(4.4, 6.6, 1.1, 2.2, 4.4, 6.6, 1, 2, 3, 4, 4)]  // Pt jj</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A34" s="42">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B34" s="43">
+        <v>6.6</v>
+      </c>
+      <c r="C34" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D34" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E34" s="42">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F34" s="43">
+        <v>6.6</v>
+      </c>
+      <c r="G34" s="42">
+        <v>1</v>
+      </c>
+      <c r="H34" s="44">
+        <v>2</v>
+      </c>
+      <c r="I34" s="44">
+        <v>3</v>
+      </c>
+      <c r="J34" s="43">
+        <v>4</v>
+      </c>
+      <c r="K34">
+        <f>(A34-C34)*(B34-D34)</f>
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <f>(E34-A34)*(B34-D34)</f>
+        <v>14.52</v>
+      </c>
+      <c r="M34">
+        <f>(A34-C34)*(F34-B34)</f>
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <f>(E34-A34)*(F34-B34)</f>
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <f>(E34-C34)*(F34-D34)</f>
+        <v>14.52</v>
+      </c>
+      <c r="P34">
+        <f>(G34*N34+H34*M34+I34*L34+J34*K34)/O34</f>
+        <v>3.0000000000000004</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>226</v>
+      </c>
+      <c r="T34" t="str">
+        <f t="shared" si="13"/>
+        <v>[TestCase(1.1, 6.6, 1.1, 2.2, 4.4, 6.6, 1, 2, 3, 4, 3)]  // Pt ij</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A35" s="42">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B35" s="43">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C35" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D35" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E35" s="42">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F35" s="43">
+        <v>6.6</v>
+      </c>
+      <c r="G35" s="42">
+        <v>1</v>
+      </c>
+      <c r="H35" s="44">
+        <v>2</v>
+      </c>
+      <c r="I35" s="44">
+        <v>3</v>
+      </c>
+      <c r="J35" s="43">
+        <v>4</v>
+      </c>
+      <c r="K35">
+        <f>(A35-C35)*(B35-D35)</f>
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <f>(E35-A35)*(B35-D35)</f>
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <f>(A35-C35)*(F35-B35)</f>
+        <v>14.52</v>
+      </c>
+      <c r="N35">
+        <f>(E35-A35)*(F35-B35)</f>
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <f>(E35-C35)*(F35-D35)</f>
+        <v>14.52</v>
+      </c>
+      <c r="P35">
+        <f>(G35*N35+H35*M35+I35*L35+J35*K35)/O35</f>
+        <v>2</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>227</v>
+      </c>
+      <c r="T35" t="str">
+        <f t="shared" si="13"/>
+        <v>[TestCase(4.4, 2.2, 1.1, 2.2, 4.4, 6.6, 1, 2, 3, 4, 2)]  // Pt ji</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A36" s="42">
+        <f>0.5*(E36-C36)+C36</f>
+        <v>2.75</v>
+      </c>
+      <c r="B36" s="43">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C36" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D36" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E36" s="42">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F36" s="43">
+        <v>6.6</v>
+      </c>
+      <c r="G36" s="42">
+        <v>1</v>
+      </c>
+      <c r="H36" s="44">
+        <v>2</v>
+      </c>
+      <c r="I36" s="44">
+        <v>3</v>
+      </c>
+      <c r="J36" s="43">
+        <v>4</v>
+      </c>
+      <c r="K36">
+        <f>(A36-C36)*(B36-D36)</f>
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <f>(E36-A36)*(B36-D36)</f>
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <f>(A36-C36)*(F36-B36)</f>
+        <v>7.2599999999999989</v>
+      </c>
+      <c r="N36">
+        <f>(E36-A36)*(F36-B36)</f>
+        <v>7.2600000000000007</v>
+      </c>
+      <c r="O36">
+        <f>(E36-C36)*(F36-D36)</f>
+        <v>14.52</v>
+      </c>
+      <c r="P36" s="3">
+        <f>(G36*N36+H36*M36+I36*L36+J36*K36)/O36</f>
+        <v>1.4999999999999998</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>221</v>
+      </c>
+      <c r="T36" t="str">
+        <f t="shared" si="13"/>
+        <v>[TestCase(2.75, 2.2, 1.1, 2.2, 4.4, 6.6, 1, 2, 3, 4, 1.5)]  // Top Edge</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A37" s="42">
+        <f>0.5*(E37-C37)+C37</f>
+        <v>2.75</v>
+      </c>
+      <c r="B37" s="43">
+        <v>6.6</v>
+      </c>
+      <c r="C37" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D37" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E37" s="42">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F37" s="43">
+        <v>6.6</v>
+      </c>
+      <c r="G37" s="42">
+        <v>1</v>
+      </c>
+      <c r="H37" s="44">
+        <v>2</v>
+      </c>
+      <c r="I37" s="44">
+        <v>3</v>
+      </c>
+      <c r="J37" s="43">
+        <v>4</v>
+      </c>
+      <c r="K37">
+        <f>(A37-C37)*(B37-D37)</f>
+        <v>7.2599999999999989</v>
+      </c>
+      <c r="L37">
+        <f>(E37-A37)*(B37-D37)</f>
+        <v>7.2600000000000007</v>
+      </c>
+      <c r="M37">
+        <f>(A37-C37)*(F37-B37)</f>
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <f>(E37-A37)*(F37-B37)</f>
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <f>(E37-C37)*(F37-D37)</f>
+        <v>14.52</v>
+      </c>
+      <c r="P37" s="3">
+        <f>(G37*N37+H37*M37+I37*L37+J37*K37)/O37</f>
+        <v>3.4999999999999996</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>231</v>
+      </c>
+      <c r="T37" t="str">
+        <f t="shared" si="13"/>
+        <v>[TestCase(2.75, 6.6, 1.1, 2.2, 4.4, 6.6, 1, 2, 3, 4, 3.5)]  // Bottom Edge</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A38" s="42">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B38" s="43">
+        <f>0.5*(F38-D38)+D38</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C38" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D38" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E38" s="42">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F38" s="43">
+        <v>6.6</v>
+      </c>
+      <c r="G38" s="42">
+        <v>1</v>
+      </c>
+      <c r="H38" s="44">
+        <v>2</v>
+      </c>
+      <c r="I38" s="44">
+        <v>3</v>
+      </c>
+      <c r="J38" s="43">
+        <v>4</v>
+      </c>
+      <c r="K38">
+        <f>(A38-C38)*(B38-D38)</f>
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <f>(E38-A38)*(B38-D38)</f>
+        <v>7.2600000000000016</v>
+      </c>
+      <c r="M38">
+        <f>(A38-C38)*(F38-B38)</f>
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <f>(E38-A38)*(F38-B38)</f>
+        <v>7.259999999999998</v>
+      </c>
+      <c r="O38">
+        <f>(E38-C38)*(F38-D38)</f>
+        <v>14.52</v>
+      </c>
+      <c r="P38" s="3">
+        <f>(G38*N38+H38*M38+I38*L38+J38*K38)/O38</f>
+        <v>2.0000000000000004</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>222</v>
+      </c>
+      <c r="T38" t="str">
+        <f t="shared" si="13"/>
+        <v>[TestCase(1.1, 4.4, 1.1, 2.2, 4.4, 6.6, 1, 2, 3, 4, 2)]  // Left Edge</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A39" s="42">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B39" s="43">
+        <f>0.5*(F39-D39)+D39</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C39" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D39" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E39" s="42">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F39" s="43">
+        <v>6.6</v>
+      </c>
+      <c r="G39" s="42">
+        <v>1</v>
+      </c>
+      <c r="H39" s="44">
+        <v>2</v>
+      </c>
+      <c r="I39" s="44">
+        <v>3</v>
+      </c>
+      <c r="J39" s="43">
+        <v>4</v>
+      </c>
+      <c r="K39">
+        <f>(A39-C39)*(B39-D39)</f>
+        <v>7.2600000000000016</v>
+      </c>
+      <c r="L39">
+        <f>(E39-A39)*(B39-D39)</f>
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <f>(A39-C39)*(F39-B39)</f>
+        <v>7.259999999999998</v>
+      </c>
+      <c r="N39">
+        <f>(E39-A39)*(F39-B39)</f>
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <f>(E39-C39)*(F39-D39)</f>
+        <v>14.52</v>
+      </c>
+      <c r="P39" s="3">
+        <f>(G39*N39+H39*M39+I39*L39+J39*K39)/O39</f>
+        <v>3.0000000000000004</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>223</v>
+      </c>
+      <c r="T39" t="str">
+        <f t="shared" si="13"/>
+        <v>[TestCase(4.4, 4.4, 1.1, 2.2, 4.4, 6.6, 1, 2, 3, 4, 3)]  // Right Edge</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A40" s="42">
+        <f>0.5*(E40-C40)+C40</f>
+        <v>2.75</v>
+      </c>
+      <c r="B40" s="43">
+        <f>0.5*(F40-D40)+D40</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C40" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D40" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E40" s="42">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F40" s="43">
+        <v>6.6</v>
+      </c>
+      <c r="G40" s="42">
+        <v>1.5</v>
+      </c>
+      <c r="H40" s="44">
+        <v>1.5</v>
+      </c>
+      <c r="I40" s="44">
+        <v>2.5</v>
+      </c>
+      <c r="J40" s="43">
+        <v>2.5</v>
+      </c>
+      <c r="K40">
+        <f>(A40-C40)*(B40-D40)</f>
+        <v>3.63</v>
+      </c>
+      <c r="L40">
+        <f>(E40-A40)*(B40-D40)</f>
+        <v>3.6300000000000012</v>
+      </c>
+      <c r="M40">
+        <f>(A40-C40)*(F40-B40)</f>
+        <v>3.6299999999999986</v>
+      </c>
+      <c r="N40">
+        <f>(E40-A40)*(F40-B40)</f>
+        <v>3.6299999999999994</v>
+      </c>
+      <c r="O40">
+        <f>(E40-C40)*(F40-D40)</f>
+        <v>14.52</v>
+      </c>
+      <c r="P40">
+        <f>(G40*N40+H40*M40+I40*L40+J40*K40)/O40</f>
+        <v>2</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>228</v>
+      </c>
+      <c r="T40" t="str">
+        <f t="shared" si="13"/>
+        <v>[TestCase(2.75, 4.4, 1.1, 2.2, 4.4, 6.6, 1.5, 1.5, 2.5, 2.5, 2)]  // Center of plane sloped along rows</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A41" s="42">
+        <f>0.5*(E41-C41)+C41</f>
+        <v>2.75</v>
+      </c>
+      <c r="B41" s="43">
+        <f>0.5*(F41-D41)+D41</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C41" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D41" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E41" s="42">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F41" s="43">
+        <v>6.6</v>
+      </c>
+      <c r="G41" s="42">
+        <v>1.5</v>
+      </c>
+      <c r="H41" s="44">
+        <v>3.5</v>
+      </c>
+      <c r="I41" s="44">
+        <v>1.5</v>
+      </c>
+      <c r="J41" s="43">
+        <v>3.5</v>
+      </c>
+      <c r="K41">
+        <f>(A41-C41)*(B41-D41)</f>
+        <v>3.63</v>
+      </c>
+      <c r="L41">
+        <f>(E41-A41)*(B41-D41)</f>
+        <v>3.6300000000000012</v>
+      </c>
+      <c r="M41">
+        <f>(A41-C41)*(F41-B41)</f>
+        <v>3.6299999999999986</v>
+      </c>
+      <c r="N41">
+        <f>(E41-A41)*(F41-B41)</f>
+        <v>3.6299999999999994</v>
+      </c>
+      <c r="O41">
+        <f>(E41-C41)*(F41-D41)</f>
+        <v>14.52</v>
+      </c>
+      <c r="P41">
+        <f>(G41*N41+H41*M41+I41*L41+J41*K41)/O41</f>
+        <v>2.5</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>229</v>
+      </c>
+      <c r="T41" t="str">
+        <f t="shared" si="13"/>
+        <v>[TestCase(2.75, 4.4, 1.1, 2.2, 4.4, 6.6, 1.5, 3.5, 1.5, 3.5, 2.5)]  // Center of plane sloped along columns</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A42" s="42">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B42" s="43">
+        <v>3.3</v>
+      </c>
+      <c r="C42" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D42" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E42" s="42">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F42" s="43">
+        <v>6.6</v>
+      </c>
+      <c r="G42" s="42">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H42" s="44">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I42" s="44">
+        <v>3.3</v>
+      </c>
+      <c r="J42" s="43">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="K42">
+        <f>(A42-C42)*(B42-D42)</f>
+        <v>1.2099999999999997</v>
+      </c>
+      <c r="L42">
+        <f>(E42-A42)*(B42-D42)</f>
+        <v>2.4199999999999995</v>
+      </c>
+      <c r="M42">
+        <f>(A42-C42)*(F42-B42)</f>
+        <v>3.63</v>
+      </c>
+      <c r="N42">
+        <f>(E42-A42)*(F42-B42)</f>
+        <v>7.26</v>
+      </c>
+      <c r="O42">
+        <f>(E42-C42)*(F42-D42)</f>
+        <v>14.52</v>
+      </c>
+      <c r="P42">
+        <f>(G42*N42+H42*M42+I42*L42+J42*K42)/O42</f>
+        <v>2.0166666666666666</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>230</v>
+      </c>
+      <c r="T42" t="str">
+        <f t="shared" si="13"/>
+        <v>[TestCase(2.2, 3.3, 1.1, 2.2, 4.4, 6.6, 1.1, 2.2, 3.3, 4.4, 2.016667)]  // All corners have different value, point not centered</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>3</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46" t="e">
+        <f>(A46-C46)*((D46-B46)/(E46-C46))+B46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G46" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>6</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="F47" t="e">
+        <f>(A47-C47)*((D47-B47)/(E47-C47))+B47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G47" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>3</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+      <c r="D48">
+        <v>6</v>
+      </c>
+      <c r="E48">
+        <v>3</v>
+      </c>
+      <c r="F48" t="e">
+        <f>(A48-C48)*((D48-B48)/(E48-C48))+B48</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G48" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>3</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49">
+        <v>10</v>
+      </c>
+      <c r="F49">
+        <f>(A49-C49)*((D49-B49)/(E49-C49))+B49</f>
+        <v>2</v>
+      </c>
+      <c r="G49" t="s">
+        <v>235</v>
+      </c>
+      <c r="I49" t="str">
+        <f>"[TestCase("&amp;A49&amp;", "&amp;B49&amp;", "&amp;C49&amp;", "&amp;D49&amp;", "&amp;E49&amp;", "&amp;ROUND(F49,6)&amp;")]  // " &amp;G49</f>
+        <v>[TestCase(3, 2, 3, 2, 10, 2)]  // vertical line</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>4</v>
+      </c>
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50">
+        <v>5</v>
+      </c>
+      <c r="E50">
+        <v>6</v>
+      </c>
+      <c r="F50">
+        <f t="shared" ref="F50:F52" si="14">(A50-C50)*((D50-B50)/(E50-C50))+B50</f>
+        <v>3</v>
+      </c>
+      <c r="G50" t="s">
+        <v>236</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" ref="I50:I52" si="15">"[TestCase("&amp;A50&amp;", "&amp;B50&amp;", "&amp;C50&amp;", "&amp;D50&amp;", "&amp;E50&amp;", "&amp;ROUND(F50,6)&amp;")]  // " &amp;G50</f>
+        <v>[TestCase(4, 2, 3, 5, 6, 3)]  // within points</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>7</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+      <c r="D51">
+        <v>5</v>
+      </c>
+      <c r="E51">
+        <v>6</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="G51" t="s">
+        <v>237</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" si="15"/>
+        <v>[TestCase(7, 2, 3, 5, 6, 6)]  // outside of points</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>-1</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52">
+        <v>-2</v>
+      </c>
+      <c r="E52">
+        <v>-3</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="14"/>
+        <v>-0.66666666666666652</v>
+      </c>
+      <c r="G52" t="s">
+        <v>239</v>
+      </c>
+      <c r="I52" t="str">
+        <f t="shared" si="15"/>
+        <v>[TestCase(-1, 2, 3, -2, -3, -0.666667)]  // negative slope</v>
       </c>
     </row>
   </sheetData>

</xml_diff>